<commit_message>
implementing foreign riders to riders list
</commit_message>
<xml_diff>
--- a/static/riders-list/RIDERS_LIST_FOR_RACE_ID-64.xlsx
+++ b/static/riders-list/RIDERS_LIST_FOR_RACE_ID-64.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ767"/>
+  <dimension ref="A1:AZ768"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -80627,6 +80627,88 @@
       </c>
       <c r="AT767" t="inlineStr"/>
     </row>
+    <row r="768">
+      <c r="A768" t="n">
+        <v>10005129361</v>
+      </c>
+      <c r="B768" t="n">
+        <v>10005129361</v>
+      </c>
+      <c r="D768" t="n">
+        <v>10005129361</v>
+      </c>
+      <c r="E768" t="n">
+        <v>10005129361</v>
+      </c>
+      <c r="F768" t="inlineStr">
+        <is>
+          <t>2022/12/31</t>
+        </is>
+      </c>
+      <c r="G768" t="inlineStr">
+        <is>
+          <t>BMX-RACE</t>
+        </is>
+      </c>
+      <c r="I768" t="inlineStr">
+        <is>
+          <t>1981/02/20</t>
+        </is>
+      </c>
+      <c r="J768" t="inlineStr">
+        <is>
+          <t>Peter</t>
+        </is>
+      </c>
+      <c r="K768" t="inlineStr">
+        <is>
+          <t>PALÁSTHY</t>
+        </is>
+      </c>
+      <c r="P768" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="Q768" t="inlineStr">
+        <is>
+          <t>Slovakia-All Clubs</t>
+        </is>
+      </c>
+      <c r="R768" t="inlineStr">
+        <is>
+          <t>SVK</t>
+        </is>
+      </c>
+      <c r="S768" t="inlineStr">
+        <is>
+          <t>CZE</t>
+        </is>
+      </c>
+      <c r="T768" t="inlineStr">
+        <is>
+          <t>Boys 11/12</t>
+        </is>
+      </c>
+      <c r="X768" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y768" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB768" t="inlineStr"/>
+      <c r="AC768" t="inlineStr"/>
+      <c r="AJ768" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="AK768" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>